<commit_message>
atp ok, ato about to implement
Signed-off-by: hkmtrhah / HKG Sherlock <hkmtrhah@gmail.com>
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18255" windowHeight="11595" tabRatio="507" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="18255" windowHeight="11595" tabRatio="507"/>
   </bookViews>
   <sheets>
     <sheet name="speed flag" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Courier New"/>
+      <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
@@ -140,18 +140,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,18 +527,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A3:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58" style="1" customWidth="1"/>
+    <col min="1" max="1" width="58" style="2" customWidth="1"/>
     <col min="5" max="5" width="26.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
@@ -554,120 +557,120 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C3,"000"),TEXT(B3,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 045000000,</v>
+      <c r="A3" s="4" t="str">
+        <f t="shared" ref="A3:A12" si="0">CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C3,"000"),TEXT(B3,"000000"),",")</f>
+        <v>0, .Beacon 8010; -1; 0; 080000000,</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 045005545,</v>
+      </c>
+      <c r="B4">
+        <v>5545</v>
+      </c>
+      <c r="C4">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C4,"000"),TEXT(B4,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 065000050,</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="C4">
-        <v>65</v>
-      </c>
-    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C5,"000"),TEXT(B5,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 080001200,</v>
+      <c r="A5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 080006025,</v>
       </c>
       <c r="B5">
-        <v>1200</v>
+        <v>6025</v>
       </c>
       <c r="C5">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C6,"000"),TEXT(B6,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 050002950,</v>
+      <c r="A6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 120008825,</v>
       </c>
       <c r="B6">
-        <v>2950</v>
+        <v>8825</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C7,"000"),TEXT(B7,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 080003850,</v>
+      <c r="A7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 080012600,</v>
       </c>
       <c r="B7">
-        <v>3850</v>
+        <v>12600</v>
       </c>
       <c r="C7">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C8,"000"),TEXT(B8,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 075005975,</v>
+      <c r="A8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 050015850,</v>
       </c>
       <c r="B8">
-        <v>5975</v>
+        <v>15850</v>
       </c>
       <c r="C8">
-        <v>75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C9,"000"),TEXT(B9,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 065007725,</v>
+      <c r="A9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 045016350,</v>
       </c>
       <c r="B9">
-        <v>7725</v>
+        <v>16350</v>
       </c>
       <c r="C9">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C10,"000"),TEXT(B10,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 080008200,</v>
+      <c r="A10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 080016850,</v>
       </c>
       <c r="B10">
-        <v>8200</v>
+        <v>16850</v>
       </c>
       <c r="C10">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C11,"000"),TEXT(B11,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 045008950,</v>
+      <c r="A11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 045021175,</v>
       </c>
       <c r="B11">
-        <v>8950</v>
+        <v>21175</v>
       </c>
       <c r="C11">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <f>CONCATENATE("0, .Beacon 8010; -1; 0; ",TEXT(C12,"000"),TEXT(B12,"000000"),",")</f>
-        <v>0, .Beacon 8010; -1; 0; 000009275,</v>
+      <c r="A12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8010; -1; 0; 000021825,</v>
       </c>
       <c r="B12">
-        <v>9275</v>
+        <v>21825</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -682,19 +685,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.75" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
@@ -705,7 +708,6 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -720,8 +722,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E3) &gt; 0, E3, "0"),", .Beacon 8020; -1; 0; ",TEXT(C3,"0"),TEXT(D3,"0"),TEXT(B3,"000000"),",")</f>
+      <c r="A3" s="4" t="str">
+        <f t="shared" ref="A3:A16" si="0">CONCATENATE(IF(COUNT(E3) &gt; 0, E3, "0"),", .Beacon 8020; -1; 0; ",TEXT(C3,"0"),TEXT(D3,"0"),TEXT(B3,"000000"),",")</f>
         <v>0, .Beacon 8020; -1; 0; 10000025,</v>
       </c>
       <c r="B3">
@@ -735,12 +737,12 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E4) &gt; 0, E4, "0"),", .Beacon 8020; -1; 0; ",TEXT(C4,"0"),TEXT(D4,"0"),TEXT(B4,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; 10000825,</v>
+      <c r="A4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10001950,</v>
       </c>
       <c r="B4">
-        <v>825</v>
+        <v>1950</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -750,12 +752,12 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E5) &gt; 0, E5, "0"),", .Beacon 8020; -1; 0; ",TEXT(C5,"0"),TEXT(D5,"0"),TEXT(B5,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; 10001750,</v>
+      <c r="A5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10003425,</v>
       </c>
       <c r="B5">
-        <v>1750</v>
+        <v>3425</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -765,12 +767,12 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E6) &gt; 0, E6, "0"),", .Beacon 8020; -1; 0; ",TEXT(C6,"0"),TEXT(D6,"0"),TEXT(B6,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; 10002950,</v>
+      <c r="A6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10004850,</v>
       </c>
       <c r="B6">
-        <v>2950</v>
+        <v>4850</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -780,130 +782,146 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E7) &gt; 0, E7, "0"),", .Beacon 8020; -1; 0; ",TEXT(C7,"0"),TEXT(D7,"0"),TEXT(B7,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; -10003400,</v>
+      <c r="A7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10005875,</v>
       </c>
       <c r="B7">
-        <v>3400</v>
+        <v>5875</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10007650,</v>
+      </c>
+      <c r="B8">
+        <v>7650</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10008950,</v>
+      </c>
+      <c r="B9">
+        <v>8950</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10012725,</v>
+      </c>
+      <c r="B10">
+        <v>12725</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; -20013725,</v>
+      </c>
+      <c r="B11">
+        <v>13725</v>
+      </c>
+      <c r="C11">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; -20015150,</v>
+      </c>
+      <c r="B12">
+        <v>15150</v>
+      </c>
+      <c r="C12">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10015825,</v>
+      </c>
+      <c r="B13">
+        <v>15825</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10019150,</v>
+      </c>
+      <c r="B14">
+        <v>19150</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 00021800,</v>
+      </c>
+      <c r="B15">
+        <v>21800</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>21450, .Beacon 8020; -1; 0; -10021800,</v>
+      </c>
+      <c r="B16">
+        <v>21800</v>
+      </c>
+      <c r="C16">
         <v>-1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E8) &gt; 0, E8, "0"),", .Beacon 8020; -1; 0; ",TEXT(C8,"0"),TEXT(D8,"0"),TEXT(B8,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; -10003850,</v>
-      </c>
-      <c r="B8">
-        <v>3850</v>
-      </c>
-      <c r="C8">
-        <v>-1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E9) &gt; 0, E9, "0"),", .Beacon 8020; -1; 0; ",TEXT(C9,"0"),TEXT(D9,"0"),TEXT(B9,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; 10004750,</v>
-      </c>
-      <c r="B9">
-        <v>4750</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E10) &gt; 0, E10, "0"),", .Beacon 8020; -1; 0; ",TEXT(C10,"0"),TEXT(D10,"0"),TEXT(B10,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; -20005450,</v>
-      </c>
-      <c r="B10">
-        <v>5450</v>
-      </c>
-      <c r="C10">
-        <v>-2</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E11) &gt; 0, E11, "0"),", .Beacon 8020; -1; 0; ",TEXT(C11,"0"),TEXT(D11,"0"),TEXT(B11,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; 10006725,</v>
-      </c>
-      <c r="B11">
-        <v>6725</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E12) &gt; 0, E12, "0"),", .Beacon 8020; -1; 0; ",TEXT(C12,"0"),TEXT(D12,"0"),TEXT(B12,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; 10007725,</v>
-      </c>
-      <c r="B12">
-        <v>7725</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E13) &gt; 0, E13, "0"),", .Beacon 8020; -1; 0; ",TEXT(C13,"0"),TEXT(D13,"0"),TEXT(B13,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; -20009250,</v>
-      </c>
-      <c r="B13">
-        <v>9250</v>
-      </c>
-      <c r="C13">
-        <v>-2</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="str">
-        <f>CONCATENATE(IF(COUNT(E14) &gt; 0, E14, "0"),", .Beacon 8020; -1; 0; ",TEXT(C14,"0"),TEXT(D14,"0"),TEXT(B14,"000000"),",")</f>
-        <v>8950, .Beacon 8020; -1; 0; 10009250,</v>
-      </c>
-      <c r="B14">
-        <v>9250</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>8950</v>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>21450</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ADD: resisting brake on up-pitch
Signed-off-by: hkgsherlock <hkgsherlock@gmail.com>
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18255" windowHeight="11595" tabRatio="507"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="8940" windowHeight="2100" tabRatio="507" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="speed flag" sheetId="1" r:id="rId1"/>
     <sheet name="stop mem" sheetId="4" r:id="rId2"/>
+    <sheet name="gradient" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Speed</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +57,13 @@
   </si>
   <si>
     <t>posToInstall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(+/-)XXXYYYYYY     X=pitch Y=trackpos</t>
+  </si>
+  <si>
+    <t>pitch (per mill)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -527,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -688,6 +696,249 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection sqref="A1:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.75" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str">
+        <f t="shared" ref="A3:A16" si="0">CONCATENATE(IF(COUNT(E3) &gt; 0, E3, "0"),", .Beacon 8020; -1; 0; ",TEXT(C3,"0"),TEXT(D3,"0"),TEXT(B3,"000000"),",")</f>
+        <v>0, .Beacon 8020; -1; 0; 10000025,</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10001950,</v>
+      </c>
+      <c r="B4">
+        <v>1950</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10003425,</v>
+      </c>
+      <c r="B5">
+        <v>3425</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10004850,</v>
+      </c>
+      <c r="B6">
+        <v>4850</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10005875,</v>
+      </c>
+      <c r="B7">
+        <v>5875</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10007650,</v>
+      </c>
+      <c r="B8">
+        <v>7650</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10008950,</v>
+      </c>
+      <c r="B9">
+        <v>8950</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10012725,</v>
+      </c>
+      <c r="B10">
+        <v>12725</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; -20013725,</v>
+      </c>
+      <c r="B11">
+        <v>13725</v>
+      </c>
+      <c r="C11">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; -20015150,</v>
+      </c>
+      <c r="B12">
+        <v>15150</v>
+      </c>
+      <c r="C12">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10015825,</v>
+      </c>
+      <c r="B13">
+        <v>15825</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 10019150,</v>
+      </c>
+      <c r="B14">
+        <v>19150</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>0, .Beacon 8020; -1; 0; 00021800,</v>
+      </c>
+      <c r="B15">
+        <v>21800</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>21450, .Beacon 8020; -1; 0; -10021800,</v>
+      </c>
+      <c r="B16">
+        <v>21800</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>21450</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -704,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,10 +963,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -723,200 +971,98 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
-        <f t="shared" ref="A3:A16" si="0">CONCATENATE(IF(COUNT(E3) &gt; 0, E3, "0"),", .Beacon 8020; -1; 0; ",TEXT(C3,"0"),TEXT(D3,"0"),TEXT(B3,"000000"),",")</f>
-        <v>0, .Beacon 8020; -1; 0; 10000025,</v>
+        <f>CONCATENATE(IF(COUNT(E3)&gt;0,E3,"0"),", .Beacon 8021; -1; 0; ",TEXT(C3,"0"),TEXT(B3,"000000"),",")</f>
+        <v>0, .Beacon 8021; -1; 0; -15000175,</v>
       </c>
       <c r="B3">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10001950,</v>
+        <f t="shared" ref="A4:A10" si="0">CONCATENATE(IF(COUNT(E4)&gt;0,E4,"0"),", .Beacon 8021; -1; 0; ",TEXT(C4,"0"),TEXT(B4,"000000"),",")</f>
+        <v>0, .Beacon 8021; -1; 0; -30000200,</v>
       </c>
       <c r="B4">
-        <v>1950</v>
+        <v>200</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10003425,</v>
+        <v>0, .Beacon 8021; -1; 0; -15000425,</v>
       </c>
       <c r="B5">
-        <v>3425</v>
+        <v>425</v>
       </c>
       <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10004850,</v>
+        <v>0, .Beacon 8021; -1; 0; 0000450,</v>
       </c>
       <c r="B6">
-        <v>4850</v>
+        <v>450</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10005875,</v>
+        <v>0, .Beacon 8021; -1; 0; 5001375,</v>
       </c>
       <c r="B7">
-        <v>5875</v>
+        <v>1375</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10007650,</v>
+        <v>0, .Beacon 8021; -1; 0; 10001400,</v>
       </c>
       <c r="B8">
-        <v>7650</v>
+        <v>1400</v>
       </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10008950,</v>
+        <v>0, .Beacon 8021; -1; 0; 5001850,</v>
       </c>
       <c r="B9">
-        <v>8950</v>
+        <v>1850</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10012725,</v>
+        <v>0, .Beacon 8021; -1; 0; 0001875,</v>
       </c>
       <c r="B10">
-        <v>12725</v>
+        <v>1875</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; -20013725,</v>
-      </c>
-      <c r="B11">
-        <v>13725</v>
-      </c>
-      <c r="C11">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; -20015150,</v>
-      </c>
-      <c r="B12">
-        <v>15150</v>
-      </c>
-      <c r="C12">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10015825,</v>
-      </c>
-      <c r="B13">
-        <v>15825</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 10019150,</v>
-      </c>
-      <c r="B14">
-        <v>19150</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>0, .Beacon 8020; -1; 0; 00021800,</v>
-      </c>
-      <c r="B15">
-        <v>21800</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>21450, .Beacon 8020; -1; 0; -10021800,</v>
-      </c>
-      <c r="B16">
-        <v>21800</v>
-      </c>
-      <c r="C16">
-        <v>-1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>21450</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>